<commit_message>
check for abbreviation before lemmatization and showing results of all folds of cross validation in table
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/context_integration/evaluation_f1_standard_deviation.xlsx
+++ b/4_classification&evaluation/output/context_integration/evaluation_f1_standard_deviation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:AQ6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,32 +436,212 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>bow</t>
+          <t>bow_mean</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>bow_chi</t>
+          <t>bow_std</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>bow_pca</t>
+          <t>bow_fold0</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>tfidf</t>
+          <t>bow_fold1</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_chi</t>
+          <t>bow_fold2</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_pca</t>
+          <t>bow_fold3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>bow_fold4</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>bow_chi_mean</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>bow_chi_std</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>bow_chi_fold0</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>bow_chi_fold1</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>bow_chi_fold2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>bow_chi_fold3</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>bow_chi_fold4</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>bow_pca_mean</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>bow_pca_std</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>bow_pca_fold0</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>bow_pca_fold1</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>bow_pca_fold2</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>bow_pca_fold3</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>bow_pca_fold4</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_mean</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_std</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_fold0</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_fold1</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_fold2</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_fold3</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_fold4</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_chi_mean</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_chi_std</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_chi_fold0</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_chi_fold1</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_chi_fold2</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_chi_fold3</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_chi_fold4</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_pca_mean</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_pca_std</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_pca_fold0</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_pca_fold1</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_pca_fold2</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_pca_fold3</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>tfidf_pca_fold4</t>
         </is>
       </c>
     </row>
@@ -472,22 +652,130 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0720654441879585</v>
+        <v>0.6695332038904875</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03832113675369622</v>
+        <v>0.07625872584471234</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03538577197691512</v>
+        <v>0.7519355693463622</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0111454688732079</v>
+        <v>0.6953776443340012</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0445273186886582</v>
+        <v>0.5247929884478258</v>
       </c>
       <c r="G2" t="n">
-        <v>0.05023123611771135</v>
+        <v>0.6865018307500879</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.6890579865741607</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.6753517827618257</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.03828838805043855</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.7267333251490277</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.6966448379012047</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.6114707338450773</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.6633033895769723</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.6786066273368463</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.6893443117370197</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.03659420154317736</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.7465792577260035</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.7079380202517599</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.6700722629763698</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.6375779671825457</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.6845540505484191</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.7906119283747787</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.01644577378844069</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.7995745458732729</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.804008406211396</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.761206341685672</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.7840602497860562</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.8042100983174962</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.7798563823293494</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.04293130496721879</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.747325109957753</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.8477890253178686</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.7260416536577039</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.804503368445506</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.7736227542679156</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.7657179631681091</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.03828221115191988</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.7235637567760038</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.8377107115247533</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.7489660482908794</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.7600258148829387</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.7583234843659706</v>
       </c>
     </row>
     <row r="3">
@@ -497,22 +785,130 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.04231474356045637</v>
+        <v>0.8185404329350711</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01747698305763679</v>
+        <v>0.05074461617514519</v>
       </c>
       <c r="D3" t="n">
-        <v>0.03640428747230327</v>
+        <v>0.7829405156532816</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0351745560024502</v>
+        <v>0.8814783433194134</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03214570763479431</v>
+        <v>0.7395328685651266</v>
       </c>
       <c r="G3" t="n">
-        <v>0.02945065064900077</v>
+        <v>0.8384812320296191</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8502692051079147</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.8232908288756373</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0201528679416892</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.802616311295768</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.8618592930137923</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.8157846651650743</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.8164487841907195</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.8197450907128326</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.815189411956425</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.03665435519781101</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.8105438323943162</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.8813542394886648</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.7709149676104829</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.8167999206500768</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.7963340996385844</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.8410460689111131</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.03706556526908131</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.8089249158347159</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.9023166360695865</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.7966939289519935</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.8480326096376449</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0.8492622540616246</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.8494769476866167</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.03328829929840962</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0.8302163015867646</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0.9023166360695865</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0.8071709071709072</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0.8372623304877711</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.8704185631180539</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0.8491655765090369</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0.03141949558899344</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.8383573388081291</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0.9023166360695865</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0.8073334309327518</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.8378646152052918</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.8599558615294256</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +918,130 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.03545215223626944</v>
+        <v>0.84132206772719</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0151915813341336</v>
+        <v>0.03032385704858274</v>
       </c>
       <c r="D4" t="n">
-        <v>0.02452466213906528</v>
+        <v>0.8526436065127723</v>
       </c>
       <c r="E4" t="n">
-        <v>0.02932135327529872</v>
+        <v>0.8800766418763024</v>
       </c>
       <c r="F4" t="n">
+        <v>0.7966196765318883</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.8167852062588905</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.8604852074560966</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.86723448644011</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.01918263765975863</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.8533676495081739</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.902639325759765</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.8607031092869015</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.848803735051613</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.8706586125940966</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.8418780221405818</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.03312118250578763</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.8435943680624531</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.902639325759765</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.8076027246758953</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.8173437390754877</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.838209953129308</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.8516567262860322</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.03125049398275771</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.8097829855514767</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.8907065946498555</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0.8495931452244342</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.8259183441282079</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.8822825618761868</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.8560758551987654</v>
+      </c>
+      <c r="AE4" t="n">
         <v>0.03625076629799822</v>
       </c>
-      <c r="G4" t="n">
-        <v>0.03625076629799822</v>
+      <c r="AF4" t="n">
+        <v>0.8097829855514767</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0.9018499948455639</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0.8495931452244342</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0.8259183441282079</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.893234806244144</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0.8580478323653455</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0.03386880377477606</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0.8196428713843776</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>0.9018499948455639</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.8495931452244342</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0.8259183441282079</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.893234806244144</v>
       </c>
     </row>
     <row r="5">
@@ -547,19 +1051,103 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.01860434227031816</v>
+        <v>0.834981754921556</v>
       </c>
       <c r="C5" t="n">
-        <v>0.01905237782978998</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
+        <v>0.02173530885574755</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.8086751274043718</v>
+      </c>
       <c r="E5" t="n">
-        <v>0.023045070544925</v>
+        <v>0.8695185908819963</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02371049052131342</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
+        <v>0.8357578776933616</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.815711612672667</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.8452455659553834</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.8482817846282467</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.02306531377168307</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.8316381460904723</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.8917888563049855</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.8464072367298173</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.8264484077897676</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.8451262762261912</v>
+      </c>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="n">
+        <v>0.8394540661465577</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.0276160274044409</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.8317763491458872</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.8812638595084207</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0.8264166328682458</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.8573123077823065</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.8005011814279279</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.8435770137537075</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0.02852401609524064</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0.8317763491458872</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>0.8919930331014809</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0.8264166328682458</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0.8573123077823065</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0.8103867458706169</v>
+      </c>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -568,22 +1156,130 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.03146725997603315</v>
+        <v>0.8493497921295168</v>
       </c>
       <c r="C6" t="n">
-        <v>0.03995425856988637</v>
+        <v>0.03695926788339739</v>
       </c>
       <c r="D6" t="n">
-        <v>0.03058982765972832</v>
+        <v>0.84005226629395</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03046994864619196</v>
+        <v>0.8909586612576383</v>
       </c>
       <c r="F6" t="n">
+        <v>0.7960007545746086</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.8286854439655799</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.8910518345558065</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.8646277994793644</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.02769932844817495</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.8514173418527545</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.9020826885106978</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.8283381697601749</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.8498009567619075</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.8914998405112869</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.836724477249097</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.02838452500014789</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.8159251487845015</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.881411330276178</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.8396132235628695</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.8481561947828667</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.7985164888390694</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.8577175509731683</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.03124491043725695</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.8721859563353505</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.9018145617000976</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0.8065672281250568</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.8475488240799434</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.8604711846253938</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.8643766410690196</v>
+      </c>
+      <c r="AE6" t="n">
         <v>0.02815255944083946</v>
       </c>
-      <c r="G6" t="n">
-        <v>0.03583863178619209</v>
+      <c r="AF6" t="n">
+        <v>0.8298521308737568</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0.9023166360695865</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0.8491090038234848</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0.8476299309066713</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0.8929755036715988</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0.8467548505383226</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.03125831068710441</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.8730625965607192</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.8808900339978232</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0.7923516095742201</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.8487425075710304</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.8387275049878201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added classification by random forest
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/context_integration/evaluation_f1_standard_deviation.xlsx
+++ b/4_classification&evaluation/output/context_integration/evaluation_f1_standard_deviation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ6"/>
+  <dimension ref="A1:AQ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -652,130 +652,130 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6695332038904875</v>
+        <v>0.6616053383069038</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07625872584471234</v>
+        <v>0.03953544260148248</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7519355693463622</v>
+        <v>0.6557244632433089</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6953776443340012</v>
+        <v>0.6046864226291436</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5247929884478258</v>
+        <v>0.6636337423737134</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6865018307500879</v>
+        <v>0.6553153359261802</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6890579865741607</v>
+        <v>0.7286667273621734</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6753517827618257</v>
+        <v>0.6814570828139329</v>
       </c>
       <c r="J2" t="n">
-        <v>0.03828838805043855</v>
+        <v>0.04100529591704264</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7267333251490277</v>
+        <v>0.6777850778042112</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6966448379012047</v>
+        <v>0.6796296017715363</v>
       </c>
       <c r="M2" t="n">
-        <v>0.6114707338450773</v>
+        <v>0.6132348862837936</v>
       </c>
       <c r="N2" t="n">
-        <v>0.6633033895769723</v>
+        <v>0.6957498402509451</v>
       </c>
       <c r="O2" t="n">
-        <v>0.6786066273368463</v>
+        <v>0.7408860079591786</v>
       </c>
       <c r="P2" t="n">
-        <v>0.6893443117370197</v>
+        <v>0.6904940944263334</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.03659420154317736</v>
+        <v>0.02497588432533826</v>
       </c>
       <c r="R2" t="n">
-        <v>0.7465792577260035</v>
+        <v>0.6700981445662297</v>
       </c>
       <c r="S2" t="n">
-        <v>0.7079380202517599</v>
+        <v>0.6752796284534057</v>
       </c>
       <c r="T2" t="n">
-        <v>0.6700722629763698</v>
+        <v>0.6834306249342563</v>
       </c>
       <c r="U2" t="n">
-        <v>0.6375779671825457</v>
+        <v>0.6843439819720654</v>
       </c>
       <c r="V2" t="n">
-        <v>0.6845540505484191</v>
+        <v>0.7393180922057093</v>
       </c>
       <c r="W2" t="n">
-        <v>0.7906119283747787</v>
+        <v>0.8018820540695701</v>
       </c>
       <c r="X2" t="n">
-        <v>0.01644577378844069</v>
+        <v>0.0352614642125757</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.7995745458732729</v>
+        <v>0.8186480186480187</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.804008406211396</v>
+        <v>0.7318755459172916</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.761206341685672</v>
+        <v>0.8273710196771193</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.7840602497860562</v>
+        <v>0.8155539649017638</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.8042100983174962</v>
+        <v>0.8159617212036567</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.7798563823293494</v>
+        <v>0.7873033124328401</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.04293130496721879</v>
+        <v>0.03297090628898847</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.747325109957753</v>
+        <v>0.7890943372748754</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.8477890253178686</v>
+        <v>0.7271889400921659</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.7260416536577039</v>
+        <v>0.8280731812989878</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.804503368445506</v>
+        <v>0.7971320171179919</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.7736227542679156</v>
+        <v>0.7950280863801797</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.7657179631681091</v>
+        <v>0.7719583017452321</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.03828221115191988</v>
+        <v>0.04306347273586575</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.7235637567760038</v>
+        <v>0.7738583246035472</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.8377107115247533</v>
+        <v>0.6928501468582939</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.7489660482908794</v>
+        <v>0.7721126899395151</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.7600258148829387</v>
+        <v>0.8150644535581287</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.7583234843659706</v>
+        <v>0.8059058937666748</v>
       </c>
     </row>
     <row r="3">
@@ -785,130 +785,130 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8185404329350711</v>
+        <v>0.814105879425558</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05074461617514519</v>
+        <v>0.0453760117518966</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7829405156532816</v>
+        <v>0.8194782168186424</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8814783433194134</v>
+        <v>0.7761646390303554</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7395328685651266</v>
+        <v>0.8191047955140237</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8384812320296191</v>
+        <v>0.7630006916933911</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8502692051079147</v>
+        <v>0.8927810540713766</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8232908288756373</v>
+        <v>0.8165697171120989</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0201528679416892</v>
+        <v>0.03696497953419494</v>
       </c>
       <c r="K3" t="n">
-        <v>0.802616311295768</v>
+        <v>0.8003224472939523</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8618592930137923</v>
+        <v>0.7677276407115117</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8157846651650743</v>
+        <v>0.8165129939323488</v>
       </c>
       <c r="N3" t="n">
-        <v>0.8164487841907195</v>
+        <v>0.8170451042371205</v>
       </c>
       <c r="O3" t="n">
-        <v>0.8197450907128326</v>
+        <v>0.8812403993855606</v>
       </c>
       <c r="P3" t="n">
-        <v>0.815189411956425</v>
+        <v>0.7882568063073884</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.03665435519781101</v>
+        <v>0.05587600468929411</v>
       </c>
       <c r="R3" t="n">
-        <v>0.8105438323943162</v>
+        <v>0.7285415219345791</v>
       </c>
       <c r="S3" t="n">
-        <v>0.8813542394886648</v>
+        <v>0.7577619238167203</v>
       </c>
       <c r="T3" t="n">
-        <v>0.7709149676104829</v>
+        <v>0.8206778005165103</v>
       </c>
       <c r="U3" t="n">
-        <v>0.8167999206500768</v>
+        <v>0.752367631741887</v>
       </c>
       <c r="V3" t="n">
-        <v>0.7963340996385844</v>
+        <v>0.8819351535272449</v>
       </c>
       <c r="W3" t="n">
-        <v>0.8410460689111131</v>
+        <v>0.86215461177632</v>
       </c>
       <c r="X3" t="n">
-        <v>0.03706556526908131</v>
+        <v>0.03596446647499382</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.8089249158347159</v>
+        <v>0.8705377220945462</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.9023166360695865</v>
+        <v>0.8166666666666667</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.7966939289519935</v>
+        <v>0.9147857424597663</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.8480326096376449</v>
+        <v>0.8275846017781501</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.8492622540616246</v>
+        <v>0.881198325882471</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.8494769476866167</v>
+        <v>0.8669515214950227</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.03328829929840962</v>
+        <v>0.03275762146175935</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.8302163015867646</v>
+        <v>0.8608829416561643</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.9023166360695865</v>
+        <v>0.8279620021555506</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.8071709071709072</v>
+        <v>0.9149881539131611</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.8372623304877711</v>
+        <v>0.8381095159320965</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.8704185631180539</v>
+        <v>0.8928149938181409</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.8491655765090369</v>
+        <v>0.8625959207273046</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.03141949558899344</v>
+        <v>0.03022425430067465</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.8383573388081291</v>
+        <v>0.8609885832900883</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.9023166360695865</v>
+        <v>0.8279620021555506</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.8073334309327518</v>
+        <v>0.9144298172415278</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.8378646152052918</v>
+        <v>0.8381095159320965</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.8599558615294256</v>
+        <v>0.8714896850172604</v>
       </c>
     </row>
     <row r="4">
@@ -918,130 +918,130 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.84132206772719</v>
+        <v>0.8484254766264593</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03032385704858274</v>
+        <v>0.04609867125037707</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8526436065127723</v>
+        <v>0.840986818030491</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8800766418763024</v>
+        <v>0.7989640892866698</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7966196765318883</v>
+        <v>0.8715139511362958</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8167852062588905</v>
+        <v>0.8060902877541248</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8604852074560966</v>
+        <v>0.9245722369247152</v>
       </c>
       <c r="I4" t="n">
-        <v>0.86723448644011</v>
+        <v>0.8715984140059622</v>
       </c>
       <c r="J4" t="n">
-        <v>0.01918263765975863</v>
+        <v>0.02798684160145205</v>
       </c>
       <c r="K4" t="n">
-        <v>0.8533676495081739</v>
+        <v>0.8621038816486616</v>
       </c>
       <c r="L4" t="n">
-        <v>0.902639325759765</v>
+        <v>0.839348103864233</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8607031092869015</v>
+        <v>0.893185533104888</v>
       </c>
       <c r="N4" t="n">
-        <v>0.848803735051613</v>
+        <v>0.849143314620146</v>
       </c>
       <c r="O4" t="n">
-        <v>0.8706586125940966</v>
+        <v>0.9142112367918819</v>
       </c>
       <c r="P4" t="n">
-        <v>0.8418780221405818</v>
+        <v>0.8548517114911736</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.03312118250578763</v>
+        <v>0.0336145026339547</v>
       </c>
       <c r="R4" t="n">
-        <v>0.8435943680624531</v>
+        <v>0.8396574107139487</v>
       </c>
       <c r="S4" t="n">
-        <v>0.902639325759765</v>
+        <v>0.8087157764577119</v>
       </c>
       <c r="T4" t="n">
-        <v>0.8076027246758953</v>
+        <v>0.8937036286740209</v>
       </c>
       <c r="U4" t="n">
-        <v>0.8173437390754877</v>
+        <v>0.8384487490868707</v>
       </c>
       <c r="V4" t="n">
-        <v>0.838209953129308</v>
+        <v>0.8937329925233151</v>
       </c>
       <c r="W4" t="n">
-        <v>0.8516567262860322</v>
+        <v>0.858065316010989</v>
       </c>
       <c r="X4" t="n">
-        <v>0.03125049398275771</v>
+        <v>0.0337552764194182</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.8097829855514767</v>
+        <v>0.828901872014974</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.8907065946498555</v>
+        <v>0.8184368867480822</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.8495931452244342</v>
+        <v>0.8702737617056016</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.8259183441282079</v>
+        <v>0.8587319843138891</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.8822825618761868</v>
+        <v>0.9139820752723978</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.8560758551987654</v>
+        <v>0.8647697933549733</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.03625076629799822</v>
+        <v>0.03275296086228412</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.8097829855514767</v>
+        <v>0.8292586277147773</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.9018499948455639</v>
+        <v>0.8281412136250846</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.8495931452244342</v>
+        <v>0.8824142817651864</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.8259183441282079</v>
+        <v>0.8700527683974202</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.893234806244144</v>
+        <v>0.9139820752723978</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.8580478323653455</v>
+        <v>0.8625653863895216</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.03386880377477606</v>
+        <v>0.03177525968687078</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.8196428713843776</v>
+        <v>0.8295415195150263</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.9018499948455639</v>
+        <v>0.8281412136250846</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.8495931452244342</v>
+        <v>0.8711093551376792</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.8259183441282079</v>
+        <v>0.8700527683974202</v>
       </c>
       <c r="AQ4" t="n">
-        <v>0.893234806244144</v>
+        <v>0.9139820752723978</v>
       </c>
     </row>
     <row r="5">
@@ -1051,46 +1051,46 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.834981754921556</v>
+        <v>0.8472833278025794</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02173530885574755</v>
+        <v>0.03531711245032959</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8086751274043718</v>
+        <v>0.8622178409412452</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8695185908819963</v>
+        <v>0.7842929818476124</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8357578776933616</v>
+        <v>0.8923855996043251</v>
       </c>
       <c r="G5" t="n">
-        <v>0.815711612672667</v>
+        <v>0.8506432054819153</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8452455659553834</v>
+        <v>0.8468770111377989</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8482817846282467</v>
+        <v>0.8604651374710626</v>
       </c>
       <c r="J5" t="n">
-        <v>0.02306531377168307</v>
+        <v>0.03408157604204808</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8316381460904723</v>
+        <v>0.8717925204812885</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8917888563049855</v>
+        <v>0.7954964390448261</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8464072367298173</v>
+        <v>0.8923855996043251</v>
       </c>
       <c r="N5" t="n">
-        <v>0.8264484077897676</v>
+        <v>0.8612331384866625</v>
       </c>
       <c r="O5" t="n">
-        <v>0.8451262762261912</v>
+        <v>0.8814179897382101</v>
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
@@ -1100,46 +1100,46 @@
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="n">
-        <v>0.8394540661465577</v>
+        <v>0.825641043605575</v>
       </c>
       <c r="X5" t="n">
-        <v>0.0276160274044409</v>
+        <v>0.04659281028642469</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.8317763491458872</v>
+        <v>0.8710619275575197</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.8812638595084207</v>
+        <v>0.7598211574247751</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.8264166328682458</v>
+        <v>0.8833409069113157</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.8573123077823065</v>
+        <v>0.7922565641995499</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.8005011814279279</v>
+        <v>0.8217246619347144</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.8435770137537075</v>
+        <v>0.8367526725646955</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.02852401609524064</v>
+        <v>0.04220680691920378</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.8317763491458872</v>
+        <v>0.8710619275575197</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.8919930331014809</v>
+        <v>0.7715930859945006</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.8264166328682458</v>
+        <v>0.892902713922485</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.8573123077823065</v>
+        <v>0.8264809734142583</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.8103867458706169</v>
+        <v>0.8217246619347144</v>
       </c>
       <c r="AK5" t="inlineStr"/>
       <c r="AL5" t="inlineStr"/>
@@ -1152,134 +1152,267 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.819964574942127</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.04345311618384834</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.7759252925486352</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.7701368405404772</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.8527884556110362</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.8182521109516017</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.8827201750588847</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.8240843164738699</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.02583954445945768</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.8138993814204805</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.8092031058578617</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.8286864918522833</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.7970157661026102</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.8716168371361133</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.7621559464350687</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.03101511909238578</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.7167428596040019</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.7434521605652489</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.8057484591709612</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.7604478265556364</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.7843884262794949</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.8047885220093512</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.031298577183661</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.756847819304923</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.7890694022909641</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0.8084289703436425</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.8183941322580603</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.8512022858491665</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.8108420237142937</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0.0362369166095132</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0.7684288219977994</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0.7994592458830108</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0.8304785865269736</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0.7850959463862689</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0.8707475177774155</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0.8191986420533903</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.0444742544506656</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.7717672373815133</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.7651082741065763</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0.8384729239289437</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.8384081491042442</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.8822366257456736</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
           <t>Ensemble</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>0.8493497921295168</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.03695926788339739</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.84005226629395</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.8909586612576383</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.7960007545746086</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.8286854439655799</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.8910518345558065</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.8646277994793644</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.02769932844817495</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.8514173418527545</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.9020826885106978</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.8283381697601749</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.8498009567619075</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.8914998405112869</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.836724477249097</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.02838452500014789</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.8159251487845015</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.881411330276178</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0.8396132235628695</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.8481561947828667</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0.7985164888390694</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0.8577175509731683</v>
-      </c>
-      <c r="X6" t="n">
-        <v>0.03124491043725695</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0.8721859563353505</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0.9018145617000976</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0.8065672281250568</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0.8475488240799434</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>0.8604711846253938</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0.8643766410690196</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>0.02815255944083946</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>0.8298521308737568</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>0.9023166360695865</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>0.8491090038234848</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>0.8476299309066713</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>0.8929755036715988</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>0.8467548505383226</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0.03125831068710441</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>0.8730625965607192</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>0.8808900339978232</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>0.7923516095742201</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>0.8487425075710304</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>0.8387275049878201</v>
+      <c r="B7" t="n">
+        <v>0.8564344881578118</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.04384619142444963</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.8305453571411018</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.8179406088324495</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.8922515656386625</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.8170073653944623</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.9244275437823826</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.8651426423712379</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.04742723010437374</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.8286217619814977</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.8084052148568277</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.9038787082748531</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.8493515848354559</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.9354559419075548</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.8346262606246398</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.04031291308432402</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.8104153356030703</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.8205516108741916</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.8106010586910417</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.8166753185507876</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.9148879794041084</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.8817900478692774</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.05025721329436046</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.8923304374134681</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.7964198251674532</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0.9356922371457135</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0.8598090431292635</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.9246986964904892</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.8620746383400251</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0.03439226246432351</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0.8281377998102392</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>0.8164417326227941</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>0.9040359635648261</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0.8705803506747646</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0.8911773450275011</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>0.8627347404167841</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0.04727350484673024</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>0.8930762530986496</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>0.7760878623357402</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>0.9146506683464736</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>0.8604164071906008</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0.8694425111124562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
metrics and f1-score standard deviation are calculated at once + separate excel files for the column charts
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/context_integration/evaluation_f1_standard_deviation.xlsx
+++ b/4_classification&evaluation/output/context_integration/evaluation_f1_standard_deviation.xlsx
@@ -541,107 +541,107 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_mean</t>
+          <t>tf-idf_mean</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_std</t>
+          <t>tf-idf_std</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_fold0</t>
+          <t>tf-idf_fold0</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_fold1</t>
+          <t>tf-idf_fold1</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_fold2</t>
+          <t>tf-idf_fold2</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_fold3</t>
+          <t>tf-idf_fold3</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_fold4</t>
+          <t>tf-idf_fold4</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_chi_mean</t>
+          <t>tf-idf_chi_mean</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_chi_std</t>
+          <t>tf-idf_chi_std</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_chi_fold0</t>
+          <t>tf-idf_chi_fold0</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_chi_fold1</t>
+          <t>tf-idf_chi_fold1</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_chi_fold2</t>
+          <t>tf-idf_chi_fold2</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_chi_fold3</t>
+          <t>tf-idf_chi_fold3</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_chi_fold4</t>
+          <t>tf-idf_chi_fold4</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_pca_mean</t>
+          <t>tf-idf_pca_mean</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_pca_std</t>
+          <t>tf-idf_pca_std</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_pca_fold0</t>
+          <t>tf-idf_pca_fold0</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_pca_fold1</t>
+          <t>tf-idf_pca_fold1</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_pca_fold2</t>
+          <t>tf-idf_pca_fold2</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_pca_fold3</t>
+          <t>tf-idf_pca_fold3</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>tfidf_pca_fold4</t>
+          <t>tf-idf_pca_fold4</t>
         </is>
       </c>
     </row>
@@ -652,25 +652,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6616053383069038</v>
+        <v>0.6499308033204485</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03953544260148248</v>
+        <v>0.05188226497714451</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6557244632433089</v>
+        <v>0.5842397836666989</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6046864226291436</v>
+        <v>0.6034764308009091</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6636337423737134</v>
+        <v>0.6685715739762719</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6553153359261802</v>
+        <v>0.6630193883996419</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7286667273621734</v>
+        <v>0.7303468397587202</v>
       </c>
       <c r="I2" t="n">
         <v>0.6814570828139329</v>
@@ -694,88 +694,88 @@
         <v>0.7408860079591786</v>
       </c>
       <c r="P2" t="n">
-        <v>0.6904940944263334</v>
+        <v>0.6868632838916314</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.02497588432533826</v>
+        <v>0.06004240274718479</v>
       </c>
       <c r="R2" t="n">
-        <v>0.6700981445662297</v>
+        <v>0.6449637123403515</v>
       </c>
       <c r="S2" t="n">
-        <v>0.6752796284534057</v>
+        <v>0.6945502170948722</v>
       </c>
       <c r="T2" t="n">
-        <v>0.6834306249342563</v>
+        <v>0.6096117951153356</v>
       </c>
       <c r="U2" t="n">
-        <v>0.6843439819720654</v>
+        <v>0.6977017551266377</v>
       </c>
       <c r="V2" t="n">
-        <v>0.7393180922057093</v>
+        <v>0.7874889397809601</v>
       </c>
       <c r="W2" t="n">
-        <v>0.8018820540695701</v>
+        <v>0.7890163061484834</v>
       </c>
       <c r="X2" t="n">
-        <v>0.0352614642125757</v>
+        <v>0.03834817423520521</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.8186480186480187</v>
+        <v>0.8072686981715195</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.7318755459172916</v>
+        <v>0.7208008256395354</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.8273710196771193</v>
+        <v>0.8371644484547711</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.8155539649017638</v>
+        <v>0.7947466475692282</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.8159617212036567</v>
+        <v>0.7851009109073626</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.7873033124328401</v>
+        <v>0.7701386303190259</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.03297090628898847</v>
+        <v>0.0606711718265975</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.7890943372748754</v>
+        <v>0.7368890352140691</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.7271889400921659</v>
+        <v>0.6678966356385712</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.8280731812989878</v>
+        <v>0.8288865256607193</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.7971320171179919</v>
+        <v>0.8235085087061239</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.7950280863801797</v>
+        <v>0.7935124463756458</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.7719583017452321</v>
+        <v>0.7747603453967136</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.04306347273586575</v>
+        <v>0.04669802744617439</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.7738583246035472</v>
+        <v>0.7747826891878354</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.6928501468582939</v>
+        <v>0.690707109042343</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.7721126899395151</v>
+        <v>0.7932054706248254</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.8150644535581287</v>
+        <v>0.8335110093312802</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.8059058937666748</v>
+        <v>0.7815954487972837</v>
       </c>
     </row>
     <row r="3">
@@ -1156,130 +1156,130 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.819964574942127</v>
+        <v>0.824133966676615</v>
       </c>
       <c r="C6" t="n">
-        <v>0.04345311618384834</v>
+        <v>0.05077201108534676</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7759252925486352</v>
+        <v>0.7786743270686259</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7701368405404772</v>
+        <v>0.7791195411464367</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8527884556110362</v>
+        <v>0.8405277892441185</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8182521109516017</v>
+        <v>0.8073995139463689</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8827201750588847</v>
+        <v>0.9149486619775244</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8240843164738699</v>
+        <v>0.8138681890195073</v>
       </c>
       <c r="J6" t="n">
-        <v>0.02583954445945768</v>
+        <v>0.05308557299049709</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8138993814204805</v>
+        <v>0.7524983176757962</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8092031058578617</v>
+        <v>0.7773160676386482</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8286864918522833</v>
+        <v>0.8394693928328861</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7970157661026102</v>
+        <v>0.7965612957123993</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8716168371361133</v>
+        <v>0.9034958712378068</v>
       </c>
       <c r="P6" t="n">
-        <v>0.7621559464350687</v>
+        <v>0.7534000713955357</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.03101511909238578</v>
+        <v>0.04603954068374024</v>
       </c>
       <c r="R6" t="n">
-        <v>0.7167428596040019</v>
+        <v>0.6976906673655618</v>
       </c>
       <c r="S6" t="n">
-        <v>0.7434521605652489</v>
+        <v>0.7235566106533849</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8057484591709612</v>
+        <v>0.7965620949047766</v>
       </c>
       <c r="U6" t="n">
-        <v>0.7604478265556364</v>
+        <v>0.7307630000803294</v>
       </c>
       <c r="V6" t="n">
-        <v>0.7843884262794949</v>
+        <v>0.8184279839736256</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8047885220093512</v>
+        <v>0.8051615125966769</v>
       </c>
       <c r="X6" t="n">
-        <v>0.031298577183661</v>
+        <v>0.02902032364832803</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.756847819304923</v>
+        <v>0.7966558937312135</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.7890694022909641</v>
+        <v>0.777177128267368</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.8084289703436425</v>
+        <v>0.7851005362500172</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.8183941322580603</v>
+        <v>0.8074180170954365</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.8512022858491665</v>
+        <v>0.8594559876393493</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.8108420237142937</v>
+        <v>0.8206418104533046</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.0362369166095132</v>
+        <v>0.0150486189466485</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.7684288219977994</v>
+        <v>0.8292955480064367</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.7994592458830108</v>
+        <v>0.7994717977740049</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.8304785865269736</v>
+        <v>0.8296687449913256</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.7850959463862689</v>
+        <v>0.8062360201579217</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.8707475177774155</v>
+        <v>0.8385369413368349</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.8191986420533903</v>
+        <v>0.8125355882640468</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.0444742544506656</v>
+        <v>0.03908838529513609</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.7717672373815133</v>
+        <v>0.7725007651058508</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.7651082741065763</v>
+        <v>0.7647826282759407</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.8384729239289437</v>
+        <v>0.8273405787045069</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.8384081491042442</v>
+        <v>0.8281230936578985</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.8822366257456736</v>
+        <v>0.8699308755760369</v>
       </c>
     </row>
     <row r="7">
@@ -1289,13 +1289,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8564344881578118</v>
+        <v>0.8542573678287834</v>
       </c>
       <c r="C7" t="n">
-        <v>0.04384619142444963</v>
+        <v>0.04194495864085813</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8305453571411018</v>
+        <v>0.8409703096153264</v>
       </c>
       <c r="E7" t="n">
         <v>0.8179406088324495</v>
@@ -1304,61 +1304,61 @@
         <v>0.8922515656386625</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8170073653944623</v>
+        <v>0.8062546772224193</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9244275437823826</v>
+        <v>0.9138696778350595</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8651426423712379</v>
+        <v>0.860939356328483</v>
       </c>
       <c r="J7" t="n">
-        <v>0.04742723010437374</v>
+        <v>0.04645641239378697</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8286217619814977</v>
+        <v>0.8297463175122749</v>
       </c>
       <c r="L7" t="n">
         <v>0.8084052148568277</v>
       </c>
       <c r="M7" t="n">
-        <v>0.9038787082748531</v>
+        <v>0.8925910075771353</v>
       </c>
       <c r="N7" t="n">
-        <v>0.8493515848354559</v>
+        <v>0.8384982997886223</v>
       </c>
       <c r="O7" t="n">
         <v>0.9354559419075548</v>
       </c>
       <c r="P7" t="n">
-        <v>0.8346262606246398</v>
+        <v>0.8282070169752302</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.04031291308432402</v>
+        <v>0.04355256613278493</v>
       </c>
       <c r="R7" t="n">
-        <v>0.8104153356030703</v>
+        <v>0.7991180662430909</v>
       </c>
       <c r="S7" t="n">
-        <v>0.8205516108741916</v>
+        <v>0.8109491118932504</v>
       </c>
       <c r="T7" t="n">
         <v>0.8106010586910417</v>
       </c>
       <c r="U7" t="n">
-        <v>0.8166753185507876</v>
+        <v>0.8054788686446601</v>
       </c>
       <c r="V7" t="n">
         <v>0.9148879794041084</v>
       </c>
       <c r="W7" t="n">
-        <v>0.8817900478692774</v>
+        <v>0.8773861715477101</v>
       </c>
       <c r="X7" t="n">
-        <v>0.05025721329436046</v>
+        <v>0.0481244053602312</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.8923304374134681</v>
+        <v>0.8820442783208741</v>
       </c>
       <c r="Z7" t="n">
         <v>0.7964198251674532</v>
@@ -1367,22 +1367,22 @@
         <v>0.9356922371457135</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.8598090431292635</v>
+        <v>0.85954598127773</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.9246986964904892</v>
+        <v>0.9132285358267801</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.8620746383400251</v>
+        <v>0.8599897504776187</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.03439226246432351</v>
+        <v>0.03728932460534133</v>
       </c>
       <c r="AF7" t="n">
         <v>0.8281377998102392</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.8164417326227941</v>
+        <v>0.806017293310763</v>
       </c>
       <c r="AH7" t="n">
         <v>0.9040359635648261</v>
@@ -1394,19 +1394,19 @@
         <v>0.8911773450275011</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.8627347404167841</v>
+        <v>0.8606441137027421</v>
       </c>
       <c r="AL7" t="n">
-        <v>0.04727350484673024</v>
+        <v>0.0452830054076079</v>
       </c>
       <c r="AM7" t="n">
-        <v>0.8930762530986496</v>
+        <v>0.8940327828905656</v>
       </c>
       <c r="AN7" t="n">
-        <v>0.7760878623357402</v>
+        <v>0.7757105750314578</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.9146506683464736</v>
+        <v>0.9036182922886306</v>
       </c>
       <c r="AP7" t="n">
         <v>0.8604164071906008</v>

</xml_diff>

<commit_message>
added tables for standard deviation of precision and recall and promise requirements as dummy data set
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/context_integration/evaluation_f1_standard_deviation.xlsx
+++ b/4_classification&evaluation/output/context_integration/evaluation_f1_standard_deviation.xlsx
@@ -1156,130 +1156,130 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.824133966676615</v>
+        <v>0.827942324055343</v>
       </c>
       <c r="C6" t="n">
-        <v>0.05077201108534676</v>
+        <v>0.02598578151053643</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7786743270686259</v>
+        <v>0.7898560923698297</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7791195411464367</v>
+        <v>0.8200384473729125</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8405277892441185</v>
+        <v>0.8294487770294222</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8073995139463689</v>
+        <v>0.8293082722044585</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9149486619775244</v>
+        <v>0.8710600313000915</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8138681890195073</v>
+        <v>0.8142274241189149</v>
       </c>
       <c r="J6" t="n">
-        <v>0.05308557299049709</v>
+        <v>0.03972142724517488</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7524983176757962</v>
+        <v>0.7654856254559372</v>
       </c>
       <c r="L6" t="n">
-        <v>0.7773160676386482</v>
+        <v>0.7886132731633581</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8394693928328861</v>
+        <v>0.828811572615664</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7965612957123993</v>
+        <v>0.8063106808976204</v>
       </c>
       <c r="O6" t="n">
-        <v>0.9034958712378068</v>
+        <v>0.8819159684619953</v>
       </c>
       <c r="P6" t="n">
-        <v>0.7534000713955357</v>
+        <v>0.7609529102436011</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.04603954068374024</v>
+        <v>0.02205912082744699</v>
       </c>
       <c r="R6" t="n">
-        <v>0.6976906673655618</v>
+        <v>0.748255198087225</v>
       </c>
       <c r="S6" t="n">
-        <v>0.7235566106533849</v>
+        <v>0.7566536360891201</v>
       </c>
       <c r="T6" t="n">
-        <v>0.7965620949047766</v>
+        <v>0.7966758337824428</v>
       </c>
       <c r="U6" t="n">
-        <v>0.7307630000803294</v>
+        <v>0.7315668202764978</v>
       </c>
       <c r="V6" t="n">
-        <v>0.8184279839736256</v>
+        <v>0.7716130629827197</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8051615125966769</v>
+        <v>0.8082327911765731</v>
       </c>
       <c r="X6" t="n">
-        <v>0.02902032364832803</v>
+        <v>0.02678402651696709</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.7966558937312135</v>
+        <v>0.7966758396235459</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.777177128267368</v>
+        <v>0.7796123624908123</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.7851005362500172</v>
+        <v>0.8301499180156344</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.8074180170954365</v>
+        <v>0.7858418975966166</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.8594559876393493</v>
+        <v>0.8488839381562563</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.8206418104533046</v>
+        <v>0.8079642493184324</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.0150486189466485</v>
+        <v>0.02998949629178382</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.8292955480064367</v>
+        <v>0.799912498848669</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.7994717977740049</v>
+        <v>0.7669725649059193</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.8296687449913256</v>
+        <v>0.8184277682672393</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.8062360201579217</v>
+        <v>0.7964482794703507</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.8385369413368349</v>
+        <v>0.8580601350999834</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.8125355882640468</v>
+        <v>0.8169122273468202</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.03908838529513609</v>
+        <v>0.04888747874274001</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.7725007651058508</v>
+        <v>0.8057839426923914</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.7647826282759407</v>
+        <v>0.7322024802100703</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.8273405787045069</v>
+        <v>0.8276870232515393</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.8281230936578985</v>
+        <v>0.8380385348127284</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.8699308755760369</v>
+        <v>0.8808491557673718</v>
       </c>
     </row>
     <row r="7">
@@ -1289,76 +1289,76 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8542573678287834</v>
+        <v>0.8526172370702561</v>
       </c>
       <c r="C7" t="n">
-        <v>0.04194495864085813</v>
+        <v>0.04726931293461654</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8409703096153264</v>
+        <v>0.8196711441392293</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8179406088324495</v>
+        <v>0.8084052148568277</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8922515656386625</v>
+        <v>0.8931043850005298</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8062546772224193</v>
+        <v>0.8170073653944623</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9138696778350595</v>
+        <v>0.9248980759602318</v>
       </c>
       <c r="I7" t="n">
-        <v>0.860939356328483</v>
+        <v>0.8715642118514711</v>
       </c>
       <c r="J7" t="n">
-        <v>0.04645641239378697</v>
+        <v>0.04207819240748639</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8297463175122749</v>
+        <v>0.8509001636661211</v>
       </c>
       <c r="L7" t="n">
-        <v>0.8084052148568277</v>
+        <v>0.818456812005199</v>
       </c>
       <c r="M7" t="n">
-        <v>0.8925910075771353</v>
+        <v>0.9036565568430243</v>
       </c>
       <c r="N7" t="n">
-        <v>0.8384982997886223</v>
+        <v>0.8493515848354559</v>
       </c>
       <c r="O7" t="n">
         <v>0.9354559419075548</v>
       </c>
       <c r="P7" t="n">
-        <v>0.8282070169752302</v>
+        <v>0.8305318399463862</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.04355256613278493</v>
+        <v>0.04252656265324263</v>
       </c>
       <c r="R7" t="n">
-        <v>0.7991180662430909</v>
+        <v>0.8106669019913335</v>
       </c>
       <c r="S7" t="n">
-        <v>0.8109491118932504</v>
+        <v>0.7998279410946603</v>
       </c>
       <c r="T7" t="n">
         <v>0.8106010586910417</v>
       </c>
       <c r="U7" t="n">
-        <v>0.8054788686446601</v>
+        <v>0.8166753185507876</v>
       </c>
       <c r="V7" t="n">
         <v>0.9148879794041084</v>
       </c>
       <c r="W7" t="n">
-        <v>0.8773861715477101</v>
+        <v>0.8795942503981061</v>
       </c>
       <c r="X7" t="n">
-        <v>0.0481244053602312</v>
+        <v>0.04652763315824815</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.8820442783208741</v>
+        <v>0.8923304374134681</v>
       </c>
       <c r="Z7" t="n">
         <v>0.7964198251674532</v>
@@ -1367,10 +1367,10 @@
         <v>0.9356922371457135</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.85954598127773</v>
+        <v>0.8710465162078066</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.9132285358267801</v>
+        <v>0.90248223605609</v>
       </c>
       <c r="AD7" t="n">
         <v>0.8599897504776187</v>
@@ -1394,25 +1394,25 @@
         <v>0.8911773450275011</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.8606441137027421</v>
+        <v>0.86305094578302</v>
       </c>
       <c r="AL7" t="n">
-        <v>0.0452830054076079</v>
+        <v>0.05070449712042256</v>
       </c>
       <c r="AM7" t="n">
-        <v>0.8940327828905656</v>
+        <v>0.9046190216402983</v>
       </c>
       <c r="AN7" t="n">
-        <v>0.7757105750314578</v>
+        <v>0.7760878623357402</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.9036182922886306</v>
+        <v>0.9146506683464736</v>
       </c>
       <c r="AP7" t="n">
-        <v>0.8604164071906008</v>
+        <v>0.8389430328946458</v>
       </c>
       <c r="AQ7" t="n">
-        <v>0.8694425111124562</v>
+        <v>0.8809541436979426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculating precision, recall and f1 score for each class label and storing them in evaluation_labels.xlsx
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/context_integration/evaluation_f1_standard_deviation.xlsx
+++ b/4_classification&evaluation/output/context_integration/evaluation_f1_standard_deviation.xlsx
@@ -1156,130 +1156,130 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.827942324055343</v>
+        <v>0.8114218564321757</v>
       </c>
       <c r="C6" t="n">
-        <v>0.02598578151053643</v>
+        <v>0.04085251278118068</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7898560923698297</v>
+        <v>0.7873104996646626</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8200384473729125</v>
+        <v>0.7598817637319197</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8294487770294222</v>
+        <v>0.8195677348903155</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8293082722044585</v>
+        <v>0.8080125380713686</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8710600313000915</v>
+        <v>0.8823367458026122</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8142274241189149</v>
+        <v>0.8103036885258821</v>
       </c>
       <c r="J6" t="n">
-        <v>0.03972142724517488</v>
+        <v>0.03220432188463117</v>
       </c>
       <c r="K6" t="n">
         <v>0.7654856254559372</v>
       </c>
       <c r="L6" t="n">
-        <v>0.7886132731633581</v>
+        <v>0.7893956922074028</v>
       </c>
       <c r="M6" t="n">
-        <v>0.828811572615664</v>
+        <v>0.8173729408977245</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8063106808976204</v>
+        <v>0.8176150098130595</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8819159684619953</v>
+        <v>0.8616491742552862</v>
       </c>
       <c r="P6" t="n">
-        <v>0.7609529102436011</v>
+        <v>0.7502166465975405</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02205912082744699</v>
+        <v>0.03802064233734331</v>
       </c>
       <c r="R6" t="n">
-        <v>0.748255198087225</v>
+        <v>0.7464301738657841</v>
       </c>
       <c r="S6" t="n">
-        <v>0.7566536360891201</v>
+        <v>0.7222977208314514</v>
       </c>
       <c r="T6" t="n">
-        <v>0.7966758337824428</v>
+        <v>0.7874027449951918</v>
       </c>
       <c r="U6" t="n">
-        <v>0.7315668202764978</v>
+        <v>0.6972955360052133</v>
       </c>
       <c r="V6" t="n">
-        <v>0.7716130629827197</v>
+        <v>0.7976570572900614</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8082327911765731</v>
+        <v>0.7996338906017397</v>
       </c>
       <c r="X6" t="n">
-        <v>0.02678402651696709</v>
+        <v>0.02091233145276001</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.7966758396235459</v>
+        <v>0.7759585813647201</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.7796123624908123</v>
+        <v>0.7885807885807886</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.8301499180156344</v>
+        <v>0.7987740915246063</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.7858418975966166</v>
+        <v>0.7965720962404345</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.8488839381562563</v>
+        <v>0.838283895298149</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.8079642493184324</v>
+        <v>0.7985360193359798</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.02998949629178382</v>
+        <v>0.02015648936769903</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.799912498848669</v>
+        <v>0.7869607982248784</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.7669725649059193</v>
+        <v>0.7865482096981149</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.8184277682672393</v>
+        <v>0.8177406822568113</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.7964482794703507</v>
+        <v>0.7744910709336025</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.8580601350999834</v>
+        <v>0.8269393355664924</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.8169122273468202</v>
+        <v>0.816752142757274</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.04888747874274001</v>
+        <v>0.04699929490164088</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.8057839426923914</v>
+        <v>0.7836641208923045</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.7322024802100703</v>
+        <v>0.7539024753446005</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.8276870232515393</v>
+        <v>0.8598590925203828</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.8380385348127284</v>
+        <v>0.8061133758714404</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.8808491557673718</v>
+        <v>0.8802216491576421</v>
       </c>
     </row>
     <row r="7">
@@ -1289,61 +1289,61 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8526172370702561</v>
+        <v>0.8546150831566068</v>
       </c>
       <c r="C7" t="n">
-        <v>0.04726931293461654</v>
+        <v>0.04171911794888308</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8196711441392293</v>
+        <v>0.8411553943468837</v>
       </c>
       <c r="E7" t="n">
         <v>0.8084052148568277</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8931043850005298</v>
+        <v>0.8922962043929785</v>
       </c>
       <c r="G7" t="n">
         <v>0.8170073653944623</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9248980759602318</v>
+        <v>0.9142112367918819</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8715642118514711</v>
+        <v>0.8733551257699386</v>
       </c>
       <c r="J7" t="n">
-        <v>0.04207819240748639</v>
+        <v>0.0446457706921685</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8509001636661211</v>
+        <v>0.8607275032806947</v>
       </c>
       <c r="L7" t="n">
-        <v>0.818456812005199</v>
+        <v>0.8179406088324495</v>
       </c>
       <c r="M7" t="n">
-        <v>0.9036565568430243</v>
+        <v>0.9141532750403719</v>
       </c>
       <c r="N7" t="n">
-        <v>0.8493515848354559</v>
+        <v>0.8384982997886223</v>
       </c>
       <c r="O7" t="n">
         <v>0.9354559419075548</v>
       </c>
       <c r="P7" t="n">
-        <v>0.8305318399463862</v>
+        <v>0.8345833091371408</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.04252656265324263</v>
+        <v>0.04033813656202853</v>
       </c>
       <c r="R7" t="n">
-        <v>0.8106669019913335</v>
+        <v>0.8115859908413101</v>
       </c>
       <c r="S7" t="n">
-        <v>0.7998279410946603</v>
+        <v>0.80934925289764</v>
       </c>
       <c r="T7" t="n">
-        <v>0.8106010586910417</v>
+        <v>0.8204180039918579</v>
       </c>
       <c r="U7" t="n">
         <v>0.8166753185507876</v>
@@ -1352,16 +1352,16 @@
         <v>0.9148879794041084</v>
       </c>
       <c r="W7" t="n">
-        <v>0.8795942503981061</v>
+        <v>0.8801393327533831</v>
       </c>
       <c r="X7" t="n">
-        <v>0.04652763315824815</v>
+        <v>0.05252221206188425</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.8923304374134681</v>
+        <v>0.8820442783208741</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.7964198251674532</v>
+        <v>0.7872149356020324</v>
       </c>
       <c r="AA7" t="n">
         <v>0.9356922371457135</v>
@@ -1370,19 +1370,19 @@
         <v>0.8710465162078066</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.90248223605609</v>
+        <v>0.9246986964904892</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.8599897504776187</v>
+        <v>0.8599540733555735</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.03728932460534133</v>
+        <v>0.03282356682811279</v>
       </c>
       <c r="AF7" t="n">
         <v>0.8281377998102392</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.806017293310763</v>
+        <v>0.8164417326227941</v>
       </c>
       <c r="AH7" t="n">
         <v>0.9040359635648261</v>
@@ -1391,25 +1391,25 @@
         <v>0.8705803506747646</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.8911773450275011</v>
+        <v>0.8805745201052426</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.86305094578302</v>
+        <v>0.8651529154314082</v>
       </c>
       <c r="AL7" t="n">
-        <v>0.05070449712042256</v>
+        <v>0.04807519083553663</v>
       </c>
       <c r="AM7" t="n">
-        <v>0.9046190216402983</v>
+        <v>0.8940327828905656</v>
       </c>
       <c r="AN7" t="n">
-        <v>0.7760878623357402</v>
+        <v>0.7757105750314578</v>
       </c>
       <c r="AO7" t="n">
         <v>0.9146506683464736</v>
       </c>
       <c r="AP7" t="n">
-        <v>0.8389430328946458</v>
+        <v>0.8604164071906008</v>
       </c>
       <c r="AQ7" t="n">
         <v>0.8809541436979426</v>

</xml_diff>